<commit_message>
Remove old Excel4 methods
</commit_message>
<xml_diff>
--- a/Handwritten/HandWritten.xlsx
+++ b/Handwritten/HandWritten.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\xlw-Examples\Handwritten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3E771F8F-13C2-41A1-A6FC-98B92B9C1388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D33071-16D5-474C-9CBB-3FAEE8B46613}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30810" yWindow="675" windowWidth="23250" windowHeight="13905"/>
+    <workbookView xWindow="660" yWindow="135" windowWidth="23250" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Concat</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Concat()</t>
   </si>
   <si>
-    <t>Concat4()</t>
-  </si>
-  <si>
     <t>Concat12()</t>
   </si>
   <si>
@@ -75,10 +72,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="183" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -121,7 +118,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -130,7 +127,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -469,11 +466,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -489,7 +486,7 @@
       </c>
       <c r="B3">
         <f ca="1">_xll.NbCalls()</f>
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>6</v>
@@ -500,11 +497,8 @@
       <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -522,19 +516,15 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
         <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
       </c>
       <c r="I4" t="str">
         <f>_xludf.Concat(G4,H4)</f>
         <v>Hello World!</v>
       </c>
-      <c r="J4" t="str">
-        <f>_xll.Concat4(G4,H4)</f>
-        <v>Hello World!</v>
-      </c>
       <c r="K4" t="str">
         <f>_xll.Concat12(G4,H4)</f>
         <v>Hello World!</v>
@@ -546,28 +536,24 @@
       </c>
       <c r="B5">
         <f t="array" aca="1" ref="B5:C5" ca="1">_xll.Stats(A9:K30)</f>
-        <v>0.51830731545010333</v>
+        <v>0.48141870924704405</v>
       </c>
       <c r="C5">
         <f ca="1"/>
-        <v>7.8888255029608279E-2</v>
+        <v>8.7969375984296966E-2</v>
       </c>
       <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
       <c r="I5" t="str">
-        <f>_xludf.Concat(G5,H5)</f>
+        <f t="array" ref="I5">_xlfn.CONCAT(G5,H5)</f>
         <v>Ahoj Světe!</v>
       </c>
-      <c r="J5" t="str">
-        <f>_xll.Concat4(G5,H5)</f>
-        <v>Ahoj Sv?te!</v>
-      </c>
       <c r="K5" t="str">
-        <f>_xll.Concat12(G5,H5)</f>
+        <f t="array" ref="K5">_xll.Concat12(G5,H5)</f>
         <v>Ahoj Světe!</v>
       </c>
     </row>
@@ -582,1023 +568,1023 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="str">
         <f ca="1">_xll.CurrentFormula()</f>
-        <v/>
+        <v>=CONCAT(RC[-2],RC[-1])</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <f t="array" ref="A9:K30" ca="1">RAND()</f>
-        <v>0.58418899673576241</v>
+        <v>0.56689841462389401</v>
       </c>
       <c r="B9" s="4">
         <f ca="1"/>
-        <v>0.38200696264899925</v>
+        <v>0.81629478603537142</v>
       </c>
       <c r="C9" s="4">
         <f ca="1"/>
-        <v>0.10592492086586824</v>
+        <v>0.99087649846964843</v>
       </c>
       <c r="D9" s="4">
         <f ca="1"/>
-        <v>0.53184361508210864</v>
+        <v>0.11225255273795143</v>
       </c>
       <c r="E9" s="4">
         <f ca="1"/>
-        <v>0.40920472908447636</v>
+        <v>0.86359728973685201</v>
       </c>
       <c r="F9" s="4">
         <f ca="1"/>
-        <v>0.87513972451556643</v>
+        <v>0.42951243888797963</v>
       </c>
       <c r="G9" s="4">
         <f ca="1"/>
-        <v>0.99943450544907519</v>
+        <v>0.33238895637575461</v>
       </c>
       <c r="H9" s="4">
         <f ca="1"/>
-        <v>0.72099601884908793</v>
+        <v>0.60680617347634835</v>
       </c>
       <c r="I9" s="4">
         <f ca="1"/>
-        <v>0.16579154443409616</v>
+        <v>1.9273517198602041E-2</v>
       </c>
       <c r="J9" s="4">
         <f ca="1"/>
-        <v>0.9956851333964033</v>
+        <v>7.1631995539414794E-2</v>
       </c>
       <c r="K9" s="4">
         <f ca="1"/>
-        <v>0.32977356943594482</v>
+        <v>0.19988605073256316</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <f ca="1"/>
-        <v>0.41194462585262015</v>
+        <v>0.26257655081379294</v>
       </c>
       <c r="B10" s="4">
         <f ca="1"/>
-        <v>0.52819117673464278</v>
+        <v>8.36740488965384E-2</v>
       </c>
       <c r="C10" s="4">
         <f ca="1"/>
-        <v>0.5403456541492675</v>
+        <v>0.72593547401107927</v>
       </c>
       <c r="D10" s="4">
         <f ca="1"/>
-        <v>0.89735006819438357</v>
+        <v>0.70610384943906701</v>
       </c>
       <c r="E10" s="4">
         <f ca="1"/>
-        <v>0.95788976322035568</v>
+        <v>0.77273410413381904</v>
       </c>
       <c r="F10" s="4">
         <f ca="1"/>
-        <v>0.55175207591830033</v>
+        <v>0.20090030900745948</v>
       </c>
       <c r="G10" s="4">
         <f ca="1"/>
-        <v>0.51553402622541711</v>
+        <v>0.19400975981653379</v>
       </c>
       <c r="H10" s="4">
         <f ca="1"/>
-        <v>0.64549228540503811</v>
+        <v>0.71929997106444798</v>
       </c>
       <c r="I10" s="4">
         <f ca="1"/>
-        <v>0.60374770560772495</v>
+        <v>0.80029808937972291</v>
       </c>
       <c r="J10" s="4">
         <f ca="1"/>
-        <v>0.94260227640236272</v>
+        <v>0.30976263091153744</v>
       </c>
       <c r="K10" s="4">
         <f ca="1"/>
-        <v>0.4366709037714227</v>
+        <v>5.7225766738861705E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <f ca="1"/>
-        <v>0.2343569581383631</v>
+        <v>8.2678569881981745E-2</v>
       </c>
       <c r="B11" s="4">
         <f ca="1"/>
-        <v>2.2053956042260126E-2</v>
+        <v>0.808817931891465</v>
       </c>
       <c r="C11" s="4">
         <f ca="1"/>
-        <v>0.3174167156570219</v>
+        <v>0.19188724969025939</v>
       </c>
       <c r="D11" s="4">
         <f ca="1"/>
-        <v>0.92853136282035531</v>
+        <v>0.95238903020886045</v>
       </c>
       <c r="E11" s="4">
         <f ca="1"/>
-        <v>0.2368287300159938</v>
+        <v>0.33268760077523585</v>
       </c>
       <c r="F11" s="4">
         <f ca="1"/>
-        <v>0.21362979736792531</v>
+        <v>0.90304212353120628</v>
       </c>
       <c r="G11" s="4">
         <f ca="1"/>
-        <v>0.96920168078155211</v>
+        <v>5.163436812908917E-2</v>
       </c>
       <c r="H11" s="4">
         <f ca="1"/>
-        <v>0.14624457218044085</v>
+        <v>0.93486758811701642</v>
       </c>
       <c r="I11" s="4">
         <f ca="1"/>
-        <v>0.21608147677589062</v>
+        <v>7.2286680528635294E-2</v>
       </c>
       <c r="J11" s="4">
         <f ca="1"/>
-        <v>0.6608046166238476</v>
+        <v>3.898932245060327E-2</v>
       </c>
       <c r="K11" s="4">
         <f ca="1"/>
-        <v>0.42601468933161746</v>
+        <v>0.18256225252030756</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <f ca="1"/>
-        <v>0.83471193938145194</v>
+        <v>0.30325891637483005</v>
       </c>
       <c r="B12" s="4">
         <f ca="1"/>
-        <v>0.65050487262875023</v>
+        <v>0.24130030413543235</v>
       </c>
       <c r="C12" s="4">
         <f ca="1"/>
-        <v>0.60524292544312019</v>
+        <v>0.66493601467838681</v>
       </c>
       <c r="D12" s="4">
         <f ca="1"/>
-        <v>0.69424434072345942</v>
+        <v>0.97477061040045032</v>
       </c>
       <c r="E12" s="4">
         <f ca="1"/>
-        <v>0.78865941858474142</v>
+        <v>0.79800341417024179</v>
       </c>
       <c r="F12" s="4">
         <f ca="1"/>
-        <v>0.88452020033777445</v>
+        <v>0.46859509716202918</v>
       </c>
       <c r="G12" s="4">
         <f ca="1"/>
-        <v>0.22362277827412691</v>
+        <v>0.99642261258981646</v>
       </c>
       <c r="H12" s="4">
         <f ca="1"/>
-        <v>0.2879270356585677</v>
+        <v>9.976485430977633E-2</v>
       </c>
       <c r="I12" s="4">
         <f ca="1"/>
-        <v>0.45589773927596955</v>
+        <v>3.3675630695213177E-2</v>
       </c>
       <c r="J12" s="4">
         <f ca="1"/>
-        <v>0.42155174293791375</v>
+        <v>0.60990241014627244</v>
       </c>
       <c r="K12" s="4">
         <f ca="1"/>
-        <v>0.9506916221190882</v>
+        <v>0.86919737737893854</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <f ca="1"/>
-        <v>0.20349225637202739</v>
+        <v>0.98526148087784016</v>
       </c>
       <c r="B13" s="4">
         <f ca="1"/>
-        <v>0.85064422866422063</v>
+        <v>0.63384455151997576</v>
       </c>
       <c r="C13" s="4">
         <f ca="1"/>
-        <v>0.62837954853467004</v>
+        <v>8.6747836158292513E-2</v>
       </c>
       <c r="D13" s="4">
         <f ca="1"/>
-        <v>0.20777306364790638</v>
+        <v>0.35098000517536032</v>
       </c>
       <c r="E13" s="4">
         <f ca="1"/>
-        <v>0.38681206592009831</v>
+        <v>0.44298250800599237</v>
       </c>
       <c r="F13" s="4">
         <f ca="1"/>
-        <v>0.26647106314852476</v>
+        <v>0.12149844910426377</v>
       </c>
       <c r="G13" s="4">
         <f ca="1"/>
-        <v>0.66301093777811515</v>
+        <v>0.85006167766266072</v>
       </c>
       <c r="H13" s="4">
         <f ca="1"/>
-        <v>0.72443457026115377</v>
+        <v>0.23044196861520638</v>
       </c>
       <c r="I13" s="4">
         <f ca="1"/>
-        <v>0.97175762999636461</v>
+        <v>0.66665396032147684</v>
       </c>
       <c r="J13" s="4">
         <f ca="1"/>
-        <v>0.65954697447818578</v>
+        <v>0.82578745660452468</v>
       </c>
       <c r="K13" s="4">
         <f ca="1"/>
-        <v>0.59097870397716701</v>
+        <v>0.10705896123480663</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <f ca="1"/>
-        <v>0.81524828048087195</v>
+        <v>0.72126363925861625</v>
       </c>
       <c r="B14" s="4">
         <f ca="1"/>
-        <v>0.40532816571478658</v>
+        <v>0.28358152895358446</v>
       </c>
       <c r="C14" s="4">
         <f ca="1"/>
-        <v>0.53969781406846018</v>
+        <v>0.18490748131896828</v>
       </c>
       <c r="D14" s="4">
         <f ca="1"/>
-        <v>0.22239463584936536</v>
+        <v>0.54787207974119756</v>
       </c>
       <c r="E14" s="4">
         <f ca="1"/>
-        <v>0.82929571861626006</v>
+        <v>0.67457040347466524</v>
       </c>
       <c r="F14" s="4">
         <f ca="1"/>
-        <v>0.88434937464646168</v>
+        <v>0.35695350471997578</v>
       </c>
       <c r="G14" s="4">
         <f ca="1"/>
-        <v>0.52494959036850386</v>
+        <v>7.9867277540878745E-2</v>
       </c>
       <c r="H14" s="4">
         <f ca="1"/>
-        <v>0.54222343874162748</v>
+        <v>0.88513353629809344</v>
       </c>
       <c r="I14" s="4">
         <f ca="1"/>
-        <v>0.1166765445701291</v>
+        <v>1.4639325601192299E-3</v>
       </c>
       <c r="J14" s="4">
         <f ca="1"/>
-        <v>0.41021220208964493</v>
+        <v>0.48355363889832326</v>
       </c>
       <c r="K14" s="4">
         <f ca="1"/>
-        <v>0.41133289821196195</v>
+        <v>0.52937560977113929</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <f ca="1"/>
-        <v>0.20919074403054716</v>
+        <v>0.76149462238704635</v>
       </c>
       <c r="B15" s="4">
         <f ca="1"/>
-        <v>0.7467877145458045</v>
+        <v>0.63447000741857096</v>
       </c>
       <c r="C15" s="4">
         <f ca="1"/>
-        <v>0.84812001023670003</v>
+        <v>0.81813951937543961</v>
       </c>
       <c r="D15" s="4">
         <f ca="1"/>
-        <v>0.82150695175945221</v>
+        <v>0.84894461879662597</v>
       </c>
       <c r="E15" s="4">
         <f ca="1"/>
-        <v>0.11584491171209887</v>
+        <v>1.2117265879961314E-2</v>
       </c>
       <c r="F15" s="4">
         <f ca="1"/>
-        <v>0.40065609574366579</v>
+        <v>0.53847984221569511</v>
       </c>
       <c r="G15" s="4">
         <f ca="1"/>
-        <v>0.37096119263178795</v>
+        <v>0.48614228683439897</v>
       </c>
       <c r="H15" s="4">
         <f ca="1"/>
-        <v>0.3262562743322347</v>
+        <v>0.46111567696456113</v>
       </c>
       <c r="I15" s="4">
         <f ca="1"/>
-        <v>0.32793109950786548</v>
+        <v>0.92779935942480274</v>
       </c>
       <c r="J15" s="4">
         <f ca="1"/>
-        <v>0.11714316157684856</v>
+        <v>0.18802267835080244</v>
       </c>
       <c r="K15" s="4">
         <f ca="1"/>
-        <v>0.80506822749287998</v>
+        <v>0.51349063613088852</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <f ca="1"/>
-        <v>7.4103768413166571E-2</v>
+        <v>0.82496412346177106</v>
       </c>
       <c r="B16" s="4">
         <f ca="1"/>
-        <v>0.19949680166790473</v>
+        <v>0.24992869775871562</v>
       </c>
       <c r="C16" s="4">
         <f ca="1"/>
-        <v>0.93619055872850643</v>
+        <v>0.40640128031676537</v>
       </c>
       <c r="D16" s="4">
         <f ca="1"/>
-        <v>0.26906266217064823</v>
+        <v>0.99035181813697482</v>
       </c>
       <c r="E16" s="4">
         <f ca="1"/>
-        <v>0.63050825208689631</v>
+        <v>0.28821635648230426</v>
       </c>
       <c r="F16" s="4">
         <f ca="1"/>
-        <v>0.21144157357736759</v>
+        <v>0.39082427411188991</v>
       </c>
       <c r="G16" s="4">
         <f ca="1"/>
-        <v>0.87156434764758384</v>
+        <v>0.45284402154829162</v>
       </c>
       <c r="H16" s="4">
         <f ca="1"/>
-        <v>0.23776032649391343</v>
+        <v>0.40855658460899369</v>
       </c>
       <c r="I16" s="4">
         <f ca="1"/>
-        <v>0.64612362934821554</v>
+        <v>0.32147560228834138</v>
       </c>
       <c r="J16" s="4">
         <f ca="1"/>
-        <v>0.6657626576833674</v>
+        <v>0.58636023618472732</v>
       </c>
       <c r="K16" s="4">
         <f ca="1"/>
-        <v>0.90181440252279987</v>
+        <v>0.74541498941658857</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <f ca="1"/>
-        <v>0.47076413806993167</v>
+        <v>0.63957136804998382</v>
       </c>
       <c r="B17" s="4">
         <f ca="1"/>
-        <v>0.77926214990320841</v>
+        <v>0.9852790050772835</v>
       </c>
       <c r="C17" s="4">
         <f ca="1"/>
-        <v>0.34313472248897747</v>
+        <v>0.41453832874441254</v>
       </c>
       <c r="D17" s="4">
         <f ca="1"/>
-        <v>0.88202171941144625</v>
+        <v>5.033504432253455E-2</v>
       </c>
       <c r="E17" s="4">
         <f ca="1"/>
-        <v>0.53421598455522579</v>
+        <v>6.8327467624520799E-2</v>
       </c>
       <c r="F17" s="4">
         <f ca="1"/>
-        <v>0.71950719191558377</v>
+        <v>0.73871573573741667</v>
       </c>
       <c r="G17" s="4">
         <f ca="1"/>
-        <v>0.15214889255624309</v>
+        <v>0.36296186702616928</v>
       </c>
       <c r="H17" s="4">
         <f ca="1"/>
-        <v>0.96794623208212505</v>
+        <v>0.491286969013221</v>
       </c>
       <c r="I17" s="4">
         <f ca="1"/>
-        <v>0.50505415956577071</v>
+        <v>0.5401964437544774</v>
       </c>
       <c r="J17" s="4">
         <f ca="1"/>
-        <v>0.53277424563808862</v>
+        <v>0.60045007011042617</v>
       </c>
       <c r="K17" s="4">
         <f ca="1"/>
-        <v>0.70965556552616915</v>
+        <v>0.82105808282924009</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <f ca="1"/>
-        <v>0.45798542164763545</v>
+        <v>0.42047628550252347</v>
       </c>
       <c r="B18" s="4">
         <f ca="1"/>
-        <v>0.84319673555527674</v>
+        <v>0.3265339906655722</v>
       </c>
       <c r="C18" s="4">
         <f ca="1"/>
-        <v>0.8064192938929674</v>
+        <v>0.53569747874867746</v>
       </c>
       <c r="D18" s="4">
         <f ca="1"/>
-        <v>0.46710134874877884</v>
+        <v>0.71047179509730085</v>
       </c>
       <c r="E18" s="4">
         <f ca="1"/>
-        <v>0.71737670428687939</v>
+        <v>0.868976203811752</v>
       </c>
       <c r="F18" s="4">
         <f ca="1"/>
-        <v>0.22477181979038696</v>
+        <v>0.38070893000527029</v>
       </c>
       <c r="G18" s="4">
         <f ca="1"/>
-        <v>0.27252041558545381</v>
+        <v>0.41664929353340396</v>
       </c>
       <c r="H18" s="4">
         <f ca="1"/>
-        <v>0.20139761386732069</v>
+        <v>0.25555274505362646</v>
       </c>
       <c r="I18" s="4">
         <f ca="1"/>
-        <v>0.71546121502674154</v>
+        <v>0.42127182319040357</v>
       </c>
       <c r="J18" s="4">
         <f ca="1"/>
-        <v>0.71283258751581946</v>
+        <v>0.3134293486502594</v>
       </c>
       <c r="K18" s="4">
         <f ca="1"/>
-        <v>0.85705462757269446</v>
+        <v>0.80456065963484569</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <f ca="1"/>
-        <v>0.2765878636457364</v>
+        <v>0.70952703564549846</v>
       </c>
       <c r="B19" s="4">
         <f ca="1"/>
-        <v>0.29276541384498145</v>
+        <v>0.31790758544080622</v>
       </c>
       <c r="C19" s="4">
         <f ca="1"/>
-        <v>0.91321816434452718</v>
+        <v>0.58842050882758223</v>
       </c>
       <c r="D19" s="4">
         <f ca="1"/>
-        <v>0.92325388412323661</v>
+        <v>0.48087766496341755</v>
       </c>
       <c r="E19" s="4">
         <f ca="1"/>
-        <v>0.92694422803662513</v>
+        <v>0.95044605378783953</v>
       </c>
       <c r="F19" s="4">
         <f ca="1"/>
-        <v>0.50647550182880363</v>
+        <v>0.81356994082698531</v>
       </c>
       <c r="G19" s="4">
         <f ca="1"/>
-        <v>0.38050879659021986</v>
+        <v>2.8827461126320064E-2</v>
       </c>
       <c r="H19" s="4">
         <f ca="1"/>
-        <v>0.7210635572181</v>
+        <v>0.99976486513466489</v>
       </c>
       <c r="I19" s="4">
         <f ca="1"/>
-        <v>0.3408459398566005</v>
+        <v>0.48568580958735486</v>
       </c>
       <c r="J19" s="4">
         <f ca="1"/>
-        <v>0.77890493512506376</v>
+        <v>0.19515583159207994</v>
       </c>
       <c r="K19" s="4">
         <f ca="1"/>
-        <v>2.975429678521202E-2</v>
+        <v>0.32031522345343055</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <f ca="1"/>
-        <v>0.63649939805664135</v>
+        <v>0.55694559839604463</v>
       </c>
       <c r="B20" s="4">
         <f ca="1"/>
-        <v>0.91396107872152321</v>
+        <v>0.81738147682608253</v>
       </c>
       <c r="C20" s="4">
         <f ca="1"/>
-        <v>0.71179034461164958</v>
+        <v>4.4398051299062713E-2</v>
       </c>
       <c r="D20" s="4">
         <f ca="1"/>
-        <v>0.50267099333261311</v>
+        <v>0.89020765181832828</v>
       </c>
       <c r="E20" s="4">
         <f ca="1"/>
-        <v>2.0243607818401288E-2</v>
+        <v>0.13844272713024219</v>
       </c>
       <c r="F20" s="4">
         <f ca="1"/>
-        <v>0.10832743317923188</v>
+        <v>0.88953886022525241</v>
       </c>
       <c r="G20" s="4">
         <f ca="1"/>
-        <v>0.2222054260655506</v>
+        <v>0.67679408362674187</v>
       </c>
       <c r="H20" s="4">
         <f ca="1"/>
-        <v>0.41161912466529793</v>
+        <v>0.55376288251041184</v>
       </c>
       <c r="I20" s="4">
         <f ca="1"/>
-        <v>0.7081774905123428</v>
+        <v>0.38037188278554024</v>
       </c>
       <c r="J20" s="4">
         <f ca="1"/>
-        <v>0.15984644527345238</v>
+        <v>6.1081148425321086E-2</v>
       </c>
       <c r="K20" s="4">
         <f ca="1"/>
-        <v>0.4992959016150359</v>
+        <v>0.66234113583409693</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <f ca="1"/>
-        <v>0.22267723698808695</v>
+        <v>0.9464672267408627</v>
       </c>
       <c r="B21" s="4">
         <f ca="1"/>
-        <v>0.41325561791827581</v>
+        <v>0.11094355334132</v>
       </c>
       <c r="C21" s="4">
         <f ca="1"/>
-        <v>0.11566814269992831</v>
+        <v>0.69628058670784054</v>
       </c>
       <c r="D21" s="4">
         <f ca="1"/>
-        <v>0.53648047386351627</v>
+        <v>0.17089156085450019</v>
       </c>
       <c r="E21" s="4">
         <f ca="1"/>
-        <v>0.68201117674395106</v>
+        <v>0.66467474747799116</v>
       </c>
       <c r="F21" s="4">
         <f ca="1"/>
-        <v>2.1949104946167308E-3</v>
+        <v>0.34679389134353689</v>
       </c>
       <c r="G21" s="4">
         <f ca="1"/>
-        <v>0.65812270682692742</v>
+        <v>0.87590700694649459</v>
       </c>
       <c r="H21" s="4">
         <f ca="1"/>
-        <v>0.34452362728397357</v>
+        <v>0.79295814597571956</v>
       </c>
       <c r="I21" s="4">
         <f ca="1"/>
-        <v>0.51140123881754984</v>
+        <v>0.54996056017537998</v>
       </c>
       <c r="J21" s="4">
         <f ca="1"/>
-        <v>4.6583494125095992E-2</v>
+        <v>0.5234403727752811</v>
       </c>
       <c r="K21" s="4">
         <f ca="1"/>
-        <v>0.75044502738705754</v>
+        <v>0.70504866561822555</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <f ca="1"/>
-        <v>0.5917739330697398</v>
+        <v>7.5510958323653288E-2</v>
       </c>
       <c r="B22" s="4">
         <f ca="1"/>
-        <v>0.23487764211936701</v>
+        <v>9.9165098073515812E-2</v>
       </c>
       <c r="C22" s="4">
         <f ca="1"/>
-        <v>0.70994485919764283</v>
+        <v>0.5744633512662406</v>
       </c>
       <c r="D22" s="4">
         <f ca="1"/>
-        <v>0.6013973423620973</v>
+        <v>0.32153651849308851</v>
       </c>
       <c r="E22" s="4">
         <f ca="1"/>
-        <v>0.52563425402990871</v>
+        <v>0.77192011425384777</v>
       </c>
       <c r="F22" s="4">
         <f ca="1"/>
-        <v>0.73222183390777973</v>
+        <v>0.75781019249747661</v>
       </c>
       <c r="G22" s="4">
         <f ca="1"/>
-        <v>0.92072294272481259</v>
+        <v>0.62526870814019597</v>
       </c>
       <c r="H22" s="4">
         <f ca="1"/>
-        <v>0.84842473235674432</v>
+        <v>0.78108387206304797</v>
       </c>
       <c r="I22" s="4">
         <f ca="1"/>
-        <v>0.68469978103860918</v>
+        <v>0.4747495366032205</v>
       </c>
       <c r="J22" s="4">
         <f ca="1"/>
-        <v>0.54389783646447976</v>
+        <v>0.16239845817502396</v>
       </c>
       <c r="K22" s="4">
         <f ca="1"/>
-        <v>0.48292089275711347</v>
+        <v>9.9620600563679162E-2</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <f ca="1"/>
-        <v>0.12856509820931838</v>
+        <v>0.64448435821170602</v>
       </c>
       <c r="B23" s="4">
         <f ca="1"/>
-        <v>0.16601968649358045</v>
+        <v>0.1896406690127721</v>
       </c>
       <c r="C23" s="4">
         <f ca="1"/>
-        <v>0.85397320094200657</v>
+        <v>6.1393964406306289E-2</v>
       </c>
       <c r="D23" s="4">
         <f ca="1"/>
-        <v>0.99478960705897146</v>
+        <v>0.77190925707375135</v>
       </c>
       <c r="E23" s="4">
         <f ca="1"/>
-        <v>0.9627231446964446</v>
+        <v>0.11853609447422719</v>
       </c>
       <c r="F23" s="4">
         <f ca="1"/>
-        <v>0.18234306444627457</v>
+        <v>0.32084363443284702</v>
       </c>
       <c r="G23" s="4">
         <f ca="1"/>
-        <v>0.88415224208273357</v>
+        <v>0.89015386858415435</v>
       </c>
       <c r="H23" s="4">
         <f ca="1"/>
-        <v>0.44843624488674583</v>
+        <v>0.74954037288543462</v>
       </c>
       <c r="I23" s="4">
         <f ca="1"/>
-        <v>0.37844861220571147</v>
+        <v>0.27710395328286097</v>
       </c>
       <c r="J23" s="4">
         <f ca="1"/>
-        <v>0.78814719210343032</v>
+        <v>0.36089110534864732</v>
       </c>
       <c r="K23" s="4">
         <f ca="1"/>
-        <v>0.80964978341177651</v>
+        <v>0.30158167831866223</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <f ca="1"/>
-        <v>0.6140403300341597</v>
+        <v>1.057354949902678E-2</v>
       </c>
       <c r="B24" s="4">
         <f ca="1"/>
-        <v>0.95573952559442898</v>
+        <v>0.35107986575781869</v>
       </c>
       <c r="C24" s="4">
         <f ca="1"/>
-        <v>7.5333552890614608E-2</v>
+        <v>0.1028061330795107</v>
       </c>
       <c r="D24" s="4">
         <f ca="1"/>
-        <v>0.12093897857298941</v>
+        <v>0.1291252508868076</v>
       </c>
       <c r="E24" s="4">
         <f ca="1"/>
-        <v>0.25076249130045458</v>
+        <v>0.32074687022988391</v>
       </c>
       <c r="F24" s="4">
         <f ca="1"/>
-        <v>0.67484368665223771</v>
+        <v>0.63739448791441844</v>
       </c>
       <c r="G24" s="4">
         <f ca="1"/>
-        <v>0.3813961454446626</v>
+        <v>0.80590060204575176</v>
       </c>
       <c r="H24" s="4">
         <f ca="1"/>
-        <v>0.95111989510510897</v>
+        <v>0.83111234273606716</v>
       </c>
       <c r="I24" s="4">
         <f ca="1"/>
-        <v>0.93000872183184136</v>
+        <v>1.2325147206489029E-2</v>
       </c>
       <c r="J24" s="4">
         <f ca="1"/>
-        <v>7.9013265248144782E-2</v>
+        <v>2.8359989629492044E-2</v>
       </c>
       <c r="K24" s="4">
         <f ca="1"/>
-        <v>0.37691398158143008</v>
+        <v>0.3643311973562019</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <f ca="1"/>
-        <v>0.61870538891880245</v>
+        <v>0.16442878768177371</v>
       </c>
       <c r="B25" s="4">
         <f ca="1"/>
-        <v>0.60419514176391365</v>
+        <v>0.84978524519567156</v>
       </c>
       <c r="C25" s="4">
         <f ca="1"/>
-        <v>0.81505306330462268</v>
+        <v>0.44590942218834728</v>
       </c>
       <c r="D25" s="4">
         <f ca="1"/>
-        <v>0.44924285978407963</v>
+        <v>0.42141828265626469</v>
       </c>
       <c r="E25" s="4">
         <f ca="1"/>
-        <v>0.65366750397515627</v>
+        <v>0.20152815395762591</v>
       </c>
       <c r="F25" s="4">
         <f ca="1"/>
-        <v>0.23916236816702519</v>
+        <v>0.35582519993944606</v>
       </c>
       <c r="G25" s="4">
         <f ca="1"/>
-        <v>0.2583721315206261</v>
+        <v>0.71943648922252557</v>
       </c>
       <c r="H25" s="4">
         <f ca="1"/>
-        <v>0.73043482062497533</v>
+        <v>0.26814631379667908</v>
       </c>
       <c r="I25" s="4">
         <f ca="1"/>
-        <v>0.21307958714260389</v>
+        <v>0.93264762901657539</v>
       </c>
       <c r="J25" s="4">
         <f ca="1"/>
-        <v>0.21058112753545055</v>
+        <v>0.90732176987311253</v>
       </c>
       <c r="K25" s="4">
         <f ca="1"/>
-        <v>0.18401416238858304</v>
+        <v>0.96365543975878198</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <f ca="1"/>
-        <v>0.14610114147791486</v>
+        <v>0.24026430876317328</v>
       </c>
       <c r="B26" s="4">
         <f ca="1"/>
-        <v>6.5446835117223268E-3</v>
+        <v>0.46371061418126269</v>
       </c>
       <c r="C26" s="4">
         <f ca="1"/>
-        <v>0.94771693442509675</v>
+        <v>0.16934227052528406</v>
       </c>
       <c r="D26" s="4">
         <f ca="1"/>
-        <v>0.55273624456696047</v>
+        <v>0.30556428313467765</v>
       </c>
       <c r="E26" s="4">
         <f ca="1"/>
-        <v>0.83626087065755839</v>
+        <v>0.60083234132509566</v>
       </c>
       <c r="F26" s="4">
         <f ca="1"/>
-        <v>0.26462428715690023</v>
+        <v>0.54728162045670914</v>
       </c>
       <c r="G26" s="4">
         <f ca="1"/>
-        <v>0.98256691185897183</v>
+        <v>0.54226675392710366</v>
       </c>
       <c r="H26" s="4">
         <f ca="1"/>
-        <v>0.25595678565151447</v>
+        <v>0.77934798228542768</v>
       </c>
       <c r="I26" s="4">
         <f ca="1"/>
-        <v>0.28754596289874856</v>
+        <v>0.62664144181427728</v>
       </c>
       <c r="J26" s="4">
         <f ca="1"/>
-        <v>0.79271963394037104</v>
+        <v>0.85885096747942979</v>
       </c>
       <c r="K26" s="4">
         <f ca="1"/>
-        <v>0.56967883728075241</v>
+        <v>6.8332714604398936E-2</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <f ca="1"/>
-        <v>0.79527765118693905</v>
+        <v>0.86932138924922364</v>
       </c>
       <c r="B27" s="4">
         <f ca="1"/>
-        <v>0.79999796233098763</v>
+        <v>5.4203042983351546E-2</v>
       </c>
       <c r="C27" s="4">
         <f ca="1"/>
-        <v>9.2630745961298944E-2</v>
+        <v>0.64748684846807747</v>
       </c>
       <c r="D27" s="4">
         <f ca="1"/>
-        <v>0.43925591195177704</v>
+        <v>0.43122146677488515</v>
       </c>
       <c r="E27" s="4">
         <f ca="1"/>
-        <v>0.69005819814213287</v>
+        <v>0.18292860853949189</v>
       </c>
       <c r="F27" s="4">
         <f ca="1"/>
-        <v>0.75870897600538112</v>
+        <v>0.95009032000227012</v>
       </c>
       <c r="G27" s="4">
         <f ca="1"/>
-        <v>0.58948658343309046</v>
+        <v>0.89571239373486766</v>
       </c>
       <c r="H27" s="4">
         <f ca="1"/>
-        <v>0.62529021509091631</v>
+        <v>0.18297389636745298</v>
       </c>
       <c r="I27" s="4">
         <f ca="1"/>
-        <v>0.13268772079292701</v>
+        <v>0.21603074291621471</v>
       </c>
       <c r="J27" s="4">
         <f ca="1"/>
-        <v>0.75946067030664766</v>
+        <v>6.7700758568602915E-2</v>
       </c>
       <c r="K27" s="4">
         <f ca="1"/>
-        <v>0.20303098831770949</v>
+        <v>0.46895276319343282</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <f ca="1"/>
-        <v>0.18047408182276725</v>
+        <v>0.19994931041782715</v>
       </c>
       <c r="B28" s="4">
         <f ca="1"/>
-        <v>0.1659178357076998</v>
+        <v>4.430704028379806E-2</v>
       </c>
       <c r="C28" s="4">
         <f ca="1"/>
-        <v>0.89797465923592501</v>
+        <v>0.79207021154923574</v>
       </c>
       <c r="D28" s="4">
         <f ca="1"/>
-        <v>0.68068389578578625</v>
+        <v>0.62079383740410654</v>
       </c>
       <c r="E28" s="4">
         <f ca="1"/>
-        <v>3.0023121626916227E-2</v>
+        <v>0.9735167828156519</v>
       </c>
       <c r="F28" s="4">
         <f ca="1"/>
-        <v>0.75985057106164877</v>
+        <v>0.44655514339728342</v>
       </c>
       <c r="G28" s="4">
         <f ca="1"/>
-        <v>0.39257316794504449</v>
+        <v>0.83945701909005588</v>
       </c>
       <c r="H28" s="4">
         <f ca="1"/>
-        <v>0.11543752330677393</v>
+        <v>0.98544506831093859</v>
       </c>
       <c r="I28" s="4">
         <f ca="1"/>
-        <v>0.83340769390384839</v>
+        <v>0.42229900209868454</v>
       </c>
       <c r="J28" s="4">
         <f ca="1"/>
-        <v>0.39311320095966618</v>
+        <v>0.1396305035237092</v>
       </c>
       <c r="K28" s="4">
         <f ca="1"/>
-        <v>0.42697237623974815</v>
+        <v>0.84315961732122113</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <f ca="1"/>
-        <v>0.37785598800074749</v>
+        <v>4.1289164941431089E-2</v>
       </c>
       <c r="B29" s="4">
         <f ca="1"/>
-        <v>0.71919043814049843</v>
+        <v>0.87198357428341156</v>
       </c>
       <c r="C29" s="4">
         <f ca="1"/>
-        <v>0.31340504565750127</v>
+        <v>0.43536294033330192</v>
       </c>
       <c r="D29" s="4">
         <f ca="1"/>
-        <v>0.79151197046578181</v>
+        <v>9.9258461039169132E-2</v>
       </c>
       <c r="E29" s="4">
         <f ca="1"/>
-        <v>0.28983811756092759</v>
+        <v>0.28176738362082365</v>
       </c>
       <c r="F29" s="4">
         <f ca="1"/>
-        <v>0.97497978965190235</v>
+        <v>8.5274608027251508E-2</v>
       </c>
       <c r="G29" s="4">
         <f ca="1"/>
-        <v>0.55197944513885289</v>
+        <v>0.37342682434911223</v>
       </c>
       <c r="H29" s="4">
         <f ca="1"/>
-        <v>0.80898225397367685</v>
+        <v>2.4211816362100569E-2</v>
       </c>
       <c r="I29" s="4">
         <f ca="1"/>
-        <v>0.97089537689077365</v>
+        <v>0.31583548916041793</v>
       </c>
       <c r="J29" s="4">
         <f ca="1"/>
-        <v>0.1988118518969374</v>
+        <v>0.5626214879367335</v>
       </c>
       <c r="K29" s="4">
         <f ca="1"/>
-        <v>0.2727752639149903</v>
+        <v>0.19286852480134975</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <f ca="1"/>
-        <v>0.29165391033496746</v>
+        <v>0.65038786198228193</v>
       </c>
       <c r="B30" s="4">
         <f ca="1"/>
-        <v>0.65997067452537561</v>
+        <v>0.82840657380183302</v>
       </c>
       <c r="C30" s="4">
         <f ca="1"/>
-        <v>0.10532493335950632</v>
+        <v>0.67748925510656832</v>
       </c>
       <c r="D30" s="4">
         <f ca="1"/>
-        <v>0.37703786177106313</v>
+        <v>0.67030085592965472</v>
       </c>
       <c r="E30" s="4">
         <f ca="1"/>
-        <v>0.16291741336307963</v>
+        <v>5.6246071786284157E-2</v>
       </c>
       <c r="F30" s="4">
         <f ca="1"/>
-        <v>0.64317326226131433</v>
+        <v>0.82813503462064553</v>
       </c>
       <c r="G30" s="4">
         <f ca="1"/>
-        <v>0.77152814275191772</v>
+        <v>0.25327929364350366</v>
       </c>
       <c r="H30" s="4">
         <f ca="1"/>
-        <v>0.22130618293396798</v>
+        <v>0.61333042757515077</v>
       </c>
       <c r="I30" s="4">
         <f ca="1"/>
-        <v>9.4137228665616246E-2</v>
+        <v>0.249668382135807</v>
       </c>
       <c r="J30" s="4">
         <f ca="1"/>
-        <v>0.5309249195290654</v>
+        <v>0.77968681207527213</v>
       </c>
       <c r="K30" s="4">
         <f ca="1"/>
-        <v>7.540780918652068E-3</v>
+        <v>0.41158728754576945</v>
       </c>
     </row>
   </sheetData>
@@ -1610,7 +1596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1624,7 +1610,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>